<commit_message>
Adds a round trip test for serialization
Modified the xlsx file to remove some metadata that Excel adds so that the round trip can get properly tested.
</commit_message>
<xml_diff>
--- a/tests/data/19_defined_names.xlsx
+++ b/tests/data/19_defined_names.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Development/xlnt/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9B1BB36-AB65-B147-A693-E8E871AE14CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="17400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="17400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,19 +17,19 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$6</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet2!$B$4</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">Sheet3!$B$2:$E$4</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$3</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">Sheet2!$A:$D</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="2">Sheet3!$B:$E,Sheet3!$2:$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet1'!$A$1:$A$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Sheet1'!$1:$3</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Sheet2'!$B$4:$B$4</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Sheet2'!$A:$D</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Sheet3'!$B$2:$E$4</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">'Sheet3'!$B:$E,'Sheet3'!$2:$4</definedName>
   </definedNames>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="150000" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -71,9 +70,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -341,8 +337,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -382,19 +380,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A6" xr:uid="{92FD0A6F-3B87-3B48-91F2-658499CB39CF}">
-    <filterColumn colId="0">
-      <customFilters>
-        <customFilter operator="greaterThan" val="3"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:A6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -409,7 +401,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>